<commit_message>
Checkin on remove dupes
</commit_message>
<xml_diff>
--- a/transformedFile.xlsx
+++ b/transformedFile.xlsx
@@ -1388,7 +1388,7 @@
         <v>vha_674 - Advice nurse</v>
       </c>
       <c r="B60" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C60" t="str">
         <v>Advice nurse at VA Central Texas health care</v>
@@ -1405,7 +1405,7 @@
         <v>vha_674 - Amputation care</v>
       </c>
       <c r="B61" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C61" t="str">
         <v>Amputation care at VA Central Texas health care</v>
@@ -1422,7 +1422,7 @@
         <v>vha_674 - Audiology and speech</v>
       </c>
       <c r="B62" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C62" t="str">
         <v>Audiology and speech at VA Central Texas health care</v>
@@ -1439,7 +1439,7 @@
         <v>vha_674 - Cardiology</v>
       </c>
       <c r="B63" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C63" t="str">
         <v>Cardiology at VA Central Texas health care</v>
@@ -1456,7 +1456,7 @@
         <v>vha_674 - Caregiver support</v>
       </c>
       <c r="B64" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C64" t="str">
         <v>Caregiver support at VA Central Texas health care</v>
@@ -1473,7 +1473,7 @@
         <v>vha_674 - Chiropractic</v>
       </c>
       <c r="B65" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C65" t="str">
         <v>Chiropractic at VA Central Texas health care</v>
@@ -1490,7 +1490,7 @@
         <v>vha_674 - Dental/oral surgery</v>
       </c>
       <c r="B66" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C66" t="str">
         <v>Dental/oral surgery at VA Central Texas health care</v>
@@ -1507,7 +1507,7 @@
         <v>vha_674 - Dermatology</v>
       </c>
       <c r="B67" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C67" t="str">
         <v>Dermatology at VA Central Texas health care</v>
@@ -1524,7 +1524,7 @@
         <v>vha_674 - Endocrinology</v>
       </c>
       <c r="B68" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C68" t="str">
         <v>Endocrinology at VA Central Texas health care</v>
@@ -1541,7 +1541,7 @@
         <v>vha_674 - Extended care and rehabilitation</v>
       </c>
       <c r="B69" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C69" t="str">
         <v>Extended care and rehabilitation at VA Central Texas health care</v>
@@ -1558,7 +1558,7 @@
         <v>vha_674 - Gastroenterology</v>
       </c>
       <c r="B70" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C70" t="str">
         <v>Gastroenterology at VA Central Texas health care</v>
@@ -1575,7 +1575,7 @@
         <v>vha_674 - Geriatrics</v>
       </c>
       <c r="B71" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C71" t="str">
         <v>Geriatrics at VA Central Texas health care</v>
@@ -1592,7 +1592,7 @@
         <v>vha_674 - Hematology/oncology</v>
       </c>
       <c r="B72" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C72" t="str">
         <v>Hematology/oncology at VA Central Texas health care</v>
@@ -1609,7 +1609,7 @@
         <v>vha_674 - Homeless Veteran care</v>
       </c>
       <c r="B73" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C73" t="str">
         <v>Homeless Veteran care at VA Central Texas health care</v>
@@ -1626,7 +1626,7 @@
         <v>vha_674 - Infectious disease</v>
       </c>
       <c r="B74" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C74" t="str">
         <v>Infectious disease at VA Central Texas health care</v>
@@ -1643,7 +1643,7 @@
         <v>vha_674 - Laboratory and pathology</v>
       </c>
       <c r="B75" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C75" t="str">
         <v>Laboratory and pathology at VA Central Texas health care</v>
@@ -1660,7 +1660,7 @@
         <v>vha_674 - LGBT Veteran care</v>
       </c>
       <c r="B76" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C76" t="str">
         <v>LGBT Veteran care at VA Central Texas health care</v>
@@ -1677,7 +1677,7 @@
         <v>vha_674 - Blind and low vision rehabilitation</v>
       </c>
       <c r="B77" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C77" t="str">
         <v>Blind and low vision rehabilitation at VA Central Texas health care</v>
@@ -1694,7 +1694,7 @@
         <v>vha_674 - Mental health care</v>
       </c>
       <c r="B78" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C78" t="str">
         <v>Mental health care at VA Central Texas health care</v>
@@ -1711,7 +1711,7 @@
         <v>vha_674 - Minority Veteran care</v>
       </c>
       <c r="B79" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C79" t="str">
         <v>Minority Veteran care at VA Central Texas health care</v>
@@ -1728,7 +1728,7 @@
         <v>vha_674 - MOVE! weight management</v>
       </c>
       <c r="B80" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C80" t="str">
         <v>MOVE! weight management at VA Central Texas health care</v>
@@ -1745,7 +1745,7 @@
         <v>vha_674 - My HealtheVet coordinator</v>
       </c>
       <c r="B81" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C81" t="str">
         <v>My HealtheVet coordinator at VA Central Texas health care</v>
@@ -1762,7 +1762,7 @@
         <v>vha_674 - Nephrology</v>
       </c>
       <c r="B82" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C82" t="str">
         <v>Nephrology at VA Central Texas health care</v>
@@ -1779,7 +1779,7 @@
         <v>vha_674 - Neurology</v>
       </c>
       <c r="B83" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C83" t="str">
         <v>Neurology at VA Central Texas health care</v>
@@ -1796,7 +1796,7 @@
         <v>vha_674 - Nutrition, food, and dietary care</v>
       </c>
       <c r="B84" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C84" t="str">
         <v>Nutrition, food, and dietary care at VA Central Texas health care</v>
@@ -1813,7 +1813,7 @@
         <v>vha_674 - Orthopedics</v>
       </c>
       <c r="B85" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C85" t="str">
         <v>Orthopedics at VA Central Texas health care</v>
@@ -1830,7 +1830,7 @@
         <v>vha_674 - Patient advocates</v>
       </c>
       <c r="B86" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C86" t="str">
         <v>Patient advocates at VA Central Texas health care</v>
@@ -1847,7 +1847,7 @@
         <v>vha_674 - Pharmacy</v>
       </c>
       <c r="B87" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C87" t="str">
         <v>Pharmacy at VA Central Texas health care</v>
@@ -1864,7 +1864,7 @@
         <v>vha_674 - Physical medicine and rehabilitation</v>
       </c>
       <c r="B88" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C88" t="str">
         <v>Physical medicine and rehabilitation at VA Central Texas health care</v>
@@ -1881,7 +1881,7 @@
         <v>vha_674 - Physical therapy, occupational therapy and kinesiotherapy</v>
       </c>
       <c r="B89" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C89" t="str">
         <v>Physical therapy, occupational therapy and kinesiotherapy at VA Central Texas health care</v>
@@ -1898,7 +1898,7 @@
         <v>vha_674 - Primary care</v>
       </c>
       <c r="B90" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C90" t="str">
         <v>Primary care at VA Central Texas health care</v>
@@ -1915,7 +1915,7 @@
         <v>vha_674 - Psychology</v>
       </c>
       <c r="B91" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C91" t="str">
         <v>Psychology at VA Central Texas health care</v>
@@ -1932,7 +1932,7 @@
         <v>vha_674 - PTSD care</v>
       </c>
       <c r="B92" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C92" t="str">
         <v>PTSD care at VA Central Texas health care</v>
@@ -1949,7 +1949,7 @@
         <v>vha_674 - Pulmonary medicine</v>
       </c>
       <c r="B93" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C93" t="str">
         <v>Pulmonary medicine at VA Central Texas health care</v>
@@ -1966,7 +1966,7 @@
         <v>vha_674 - Recreation and creative arts therapy</v>
       </c>
       <c r="B94" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C94" t="str">
         <v>Recreation and creative arts therapy at VA Central Texas health care</v>
@@ -1983,7 +1983,7 @@
         <v>vha_674 - Rehabilitation and prosthetics</v>
       </c>
       <c r="B95" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C95" t="str">
         <v>Rehabilitation and prosthetics at VA Central Texas health care</v>
@@ -2000,7 +2000,7 @@
         <v>vha_674 - Returning service member care</v>
       </c>
       <c r="B96" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C96" t="str">
         <v>Returning service member care at VA Central Texas health care</v>
@@ -2017,7 +2017,7 @@
         <v>vha_674 - Rheumatology</v>
       </c>
       <c r="B97" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C97" t="str">
         <v>Rheumatology at VA Central Texas health care</v>
@@ -2034,7 +2034,7 @@
         <v>vha_674 - Social work</v>
       </c>
       <c r="B98" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C98" t="str">
         <v>Social work at VA Central Texas health care</v>
@@ -2051,7 +2051,7 @@
         <v>vha_674 - Spinal cord injury and disorders</v>
       </c>
       <c r="B99" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C99" t="str">
         <v>Spinal cord injury and disorders at VA Central Texas health care</v>
@@ -2068,7 +2068,7 @@
         <v>vha_674 - Suicide prevention</v>
       </c>
       <c r="B100" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C100" t="str">
         <v>Suicide prevention at VA Central Texas health care</v>
@@ -2085,7 +2085,7 @@
         <v>vha_674 - Telehealth</v>
       </c>
       <c r="B101" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C101" t="str">
         <v>Telehealth at VA Central Texas health care</v>
@@ -2102,7 +2102,7 @@
         <v>vha_674 - Women Veteran care</v>
       </c>
       <c r="B102" t="str">
-        <v>Olin E. Teague Veterans' Center</v>
+        <v>Olin E. Teague Veterans Center</v>
       </c>
       <c r="C102" t="str">
         <v>Women Veteran care at VA Central Texas health care</v>
@@ -5434,7 +5434,7 @@
         <v>vha_671 - Allergy, asthma and immunology</v>
       </c>
       <c r="B298" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C298" t="str">
         <v>Allergy, asthma and immunology at VA South Texas health care</v>
@@ -5451,7 +5451,7 @@
         <v>vha_671 - Audiology and speech</v>
       </c>
       <c r="B299" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C299" t="str">
         <v>Audiology and speech at VA South Texas health care</v>
@@ -5468,7 +5468,7 @@
         <v>vha_671 - Cancer care</v>
       </c>
       <c r="B300" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C300" t="str">
         <v>Cancer care at VA South Texas health care</v>
@@ -5485,7 +5485,7 @@
         <v>vha_671 - Cardiology</v>
       </c>
       <c r="B301" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C301" t="str">
         <v>Cardiology at VA South Texas health care</v>
@@ -5502,7 +5502,7 @@
         <v>vha_671 - Caregiver support</v>
       </c>
       <c r="B302" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C302" t="str">
         <v>Caregiver support at VA South Texas health care</v>
@@ -5519,7 +5519,7 @@
         <v>vha_671 - Critical care</v>
       </c>
       <c r="B303" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C303" t="str">
         <v>Critical care at VA South Texas health care</v>
@@ -5536,7 +5536,7 @@
         <v>vha_671 - Dental/oral surgery</v>
       </c>
       <c r="B304" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C304" t="str">
         <v>Dental/oral surgery at VA South Texas health care</v>
@@ -5553,7 +5553,7 @@
         <v>vha_671 - Dermatology</v>
       </c>
       <c r="B305" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C305" t="str">
         <v>Dermatology at VA South Texas health care</v>
@@ -5570,7 +5570,7 @@
         <v>vha_671 - Endocrinology</v>
       </c>
       <c r="B306" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C306" t="str">
         <v>Endocrinology at VA South Texas health care</v>
@@ -5587,7 +5587,7 @@
         <v>vha_671 - Extended care and rehabilitation</v>
       </c>
       <c r="B307" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C307" t="str">
         <v>Extended care and rehabilitation at VA South Texas health care</v>
@@ -5604,7 +5604,7 @@
         <v>vha_671 - Gastroenterology</v>
       </c>
       <c r="B308" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C308" t="str">
         <v>Gastroenterology at VA South Texas health care</v>
@@ -5621,7 +5621,7 @@
         <v>vha_671 - Geriatrics</v>
       </c>
       <c r="B309" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C309" t="str">
         <v>Geriatrics at VA South Texas health care</v>
@@ -5638,7 +5638,7 @@
         <v>vha_671 - Hematology/oncology</v>
       </c>
       <c r="B310" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C310" t="str">
         <v>Hematology/oncology at VA South Texas health care</v>
@@ -5655,7 +5655,7 @@
         <v>vha_671 - Homeless Veteran care</v>
       </c>
       <c r="B311" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C311" t="str">
         <v>Homeless Veteran care at VA South Texas health care</v>
@@ -5672,7 +5672,7 @@
         <v>vha_671 - Infectious disease</v>
       </c>
       <c r="B312" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C312" t="str">
         <v>Infectious disease at VA South Texas health care</v>
@@ -5689,7 +5689,7 @@
         <v>vha_671 - LGBT Veteran care</v>
       </c>
       <c r="B313" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C313" t="str">
         <v>LGBT Veteran care at VA South Texas health care</v>
@@ -5706,7 +5706,7 @@
         <v>vha_671 - Blind and low vision rehabilitation</v>
       </c>
       <c r="B314" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C314" t="str">
         <v>Blind and low vision rehabilitation at VA South Texas health care</v>
@@ -5723,7 +5723,7 @@
         <v>vha_671 - Mental health care</v>
       </c>
       <c r="B315" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C315" t="str">
         <v>Mental health care at VA South Texas health care</v>
@@ -5740,7 +5740,7 @@
         <v>vha_671 - Military sexual trauma care</v>
       </c>
       <c r="B316" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C316" t="str">
         <v>Military sexual trauma care at VA South Texas health care</v>
@@ -5757,7 +5757,7 @@
         <v>vha_671 - Minority Veteran care</v>
       </c>
       <c r="B317" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C317" t="str">
         <v>Minority Veteran care at VA South Texas health care</v>
@@ -5774,7 +5774,7 @@
         <v>vha_671 - MOVE! weight management</v>
       </c>
       <c r="B318" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C318" t="str">
         <v>MOVE! weight management at VA South Texas health care</v>
@@ -5791,7 +5791,7 @@
         <v>vha_671 - Nephrology</v>
       </c>
       <c r="B319" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C319" t="str">
         <v>Nephrology at VA South Texas health care</v>
@@ -5808,7 +5808,7 @@
         <v>vha_671 - Neurology</v>
       </c>
       <c r="B320" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C320" t="str">
         <v>Neurology at VA South Texas health care</v>
@@ -5825,7 +5825,7 @@
         <v>vha_671 - Palliative and hospice care</v>
       </c>
       <c r="B321" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C321" t="str">
         <v>Palliative and hospice care at VA South Texas health care</v>
@@ -5842,7 +5842,7 @@
         <v>vha_671 - Patient advocates</v>
       </c>
       <c r="B322" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C322" t="str">
         <v>Patient advocates at VA South Texas health care</v>
@@ -5859,7 +5859,7 @@
         <v>vha_671 - Pharmacy</v>
       </c>
       <c r="B323" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C323" t="str">
         <v>Pharmacy at VA South Texas health care</v>
@@ -5876,7 +5876,7 @@
         <v>vha_671 - Physical medicine and rehabilitation</v>
       </c>
       <c r="B324" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C324" t="str">
         <v>Physical medicine and rehabilitation at VA South Texas health care</v>
@@ -5893,7 +5893,7 @@
         <v>vha_671 - Polytrauma and traumatic brain injury</v>
       </c>
       <c r="B325" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C325" t="str">
         <v>Polytrauma and traumatic brain injury at VA South Texas health care</v>
@@ -5910,7 +5910,7 @@
         <v>vha_671 - Primary care</v>
       </c>
       <c r="B326" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C326" t="str">
         <v>Primary care at VA South Texas health care</v>
@@ -5927,7 +5927,7 @@
         <v>vha_671 - Pulmonary medicine</v>
       </c>
       <c r="B327" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C327" t="str">
         <v>Pulmonary medicine at VA South Texas health care</v>
@@ -5944,7 +5944,7 @@
         <v>vha_671 - Rehabilitation and prosthetics</v>
       </c>
       <c r="B328" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C328" t="str">
         <v>Rehabilitation and prosthetics at VA South Texas health care</v>
@@ -5961,7 +5961,7 @@
         <v>vha_671 - Returning service member care</v>
       </c>
       <c r="B329" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C329" t="str">
         <v>Returning service member care at VA South Texas health care</v>
@@ -5978,7 +5978,7 @@
         <v>vha_671 - Rheumatology</v>
       </c>
       <c r="B330" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C330" t="str">
         <v>Rheumatology at VA South Texas health care</v>
@@ -5995,7 +5995,7 @@
         <v>vha_671 - Sleep medicine</v>
       </c>
       <c r="B331" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C331" t="str">
         <v>Sleep medicine at VA South Texas health care</v>
@@ -6012,7 +6012,7 @@
         <v>vha_671 - Social work</v>
       </c>
       <c r="B332" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C332" t="str">
         <v>Social work at VA South Texas health care</v>
@@ -6029,7 +6029,7 @@
         <v>vha_671 - Suicide prevention</v>
       </c>
       <c r="B333" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C333" t="str">
         <v>Suicide prevention at VA South Texas health care</v>
@@ -6046,7 +6046,7 @@
         <v>vha_671 - Telehealth</v>
       </c>
       <c r="B334" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C334" t="str">
         <v>Telehealth at VA South Texas health care</v>
@@ -6063,7 +6063,7 @@
         <v>vha_671 - Transplant surgery</v>
       </c>
       <c r="B335" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C335" t="str">
         <v>Transplant surgery at VA South Texas health care</v>
@@ -6080,7 +6080,7 @@
         <v>vha_671 - Vocational rehabilitation and employment programs</v>
       </c>
       <c r="B336" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C336" t="str">
         <v>Vocational rehabilitation and employment programs at VA South Texas health care</v>
@@ -6097,7 +6097,7 @@
         <v>vha_671 - Women Veteran care</v>
       </c>
       <c r="B337" t="str">
-        <v>Audie L. Murphy Memorial Veterans' Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans Hospital</v>
       </c>
       <c r="C337" t="str">
         <v>Women Veteran care at VA South Texas health care</v>
@@ -9582,7 +9582,7 @@
         <v>vha_519 - Addiction and substance abuse care</v>
       </c>
       <c r="B542" t="str">
-        <v>George H. O'Brien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C542" t="str">
         <v>Addiction and substance abuse care at VA West Texas health care</v>
@@ -9599,7 +9599,7 @@
         <v>vha_519 - Advice nurse</v>
       </c>
       <c r="B543" t="str">
-        <v>George H. O'Brien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C543" t="str">
         <v>Advice nurse at VA West Texas health care</v>
@@ -9616,7 +9616,7 @@
         <v>vha_519 - Audiology and speech</v>
       </c>
       <c r="B544" t="str">
-        <v>George H. O'Brien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C544" t="str">
         <v>Audiology and speech at VA West Texas health care</v>
@@ -9633,7 +9633,7 @@
         <v>vha_519 - Caregiver support</v>
       </c>
       <c r="B545" t="str">
-        <v>George H. O'Brien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C545" t="str">
         <v>Caregiver support at VA West Texas health care</v>
@@ -9650,7 +9650,7 @@
         <v>vha_519 - Dental/oral surgery</v>
       </c>
       <c r="B546" t="str">
-        <v>George H. O'Brien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C546" t="str">
         <v>Dental/oral surgery at VA West Texas health care</v>
@@ -9667,7 +9667,7 @@
         <v>vha_519 - Extended care and rehabilitation</v>
       </c>
       <c r="B547" t="str">
-        <v>George H. O'Brien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C547" t="str">
         <v>Extended care and rehabilitation at VA West Texas health care</v>
@@ -9684,7 +9684,7 @@
         <v>vha_519 - Homeless Veteran care</v>
       </c>
       <c r="B548" t="str">
-        <v>George H. O'Brien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C548" t="str">
         <v>Homeless Veteran care at VA West Texas health care</v>
@@ -9701,7 +9701,7 @@
         <v>vha_519 - Laboratory and pathology</v>
       </c>
       <c r="B549" t="str">
-        <v>George H. O'Brien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C549" t="str">
         <v>Laboratory and pathology at VA West Texas health care</v>
@@ -9718,7 +9718,7 @@
         <v>vha_519 - LGBT Veteran care</v>
       </c>
       <c r="B550" t="str">
-        <v>George H. O'Brien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C550" t="str">
         <v>LGBT Veteran care at VA West Texas health care</v>
@@ -9735,7 +9735,7 @@
         <v>vha_519 - Mental health care</v>
       </c>
       <c r="B551" t="str">
-        <v>George H. O'Brien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C551" t="str">
         <v>Mental health care at VA West Texas health care</v>
@@ -9752,7 +9752,7 @@
         <v>vha_519 - Minority Veteran care</v>
       </c>
       <c r="B552" t="str">
-        <v>George H. O'Brien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C552" t="str">
         <v>Minority Veteran care at VA West Texas health care</v>
@@ -9769,7 +9769,7 @@
         <v>vha_519 - Nutrition, food, and dietary care</v>
       </c>
       <c r="B553" t="str">
-        <v>George H. O'Brien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C553" t="str">
         <v>Nutrition, food, and dietary care at VA West Texas health care</v>
@@ -9786,7 +9786,7 @@
         <v>vha_519 - Ophthalmology</v>
       </c>
       <c r="B554" t="str">
-        <v>George H. O'Brien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C554" t="str">
         <v>Ophthalmology at VA West Texas health care</v>
@@ -9803,7 +9803,7 @@
         <v>vha_519 - Palliative and hospice care</v>
       </c>
       <c r="B555" t="str">
-        <v>George H. O'Brien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C555" t="str">
         <v>Palliative and hospice care at VA West Texas health care</v>
@@ -9820,7 +9820,7 @@
         <v>vha_519 - Patient advocates</v>
       </c>
       <c r="B556" t="str">
-        <v>George H. O'Brien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C556" t="str">
         <v>Patient advocates at VA West Texas health care</v>
@@ -9837,7 +9837,7 @@
         <v>vha_519 - Pharmacy</v>
       </c>
       <c r="B557" t="str">
-        <v>George H. O'Brien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C557" t="str">
         <v>Pharmacy at VA West Texas health care</v>
@@ -9854,7 +9854,7 @@
         <v>vha_519 - Physical medicine and rehabilitation</v>
       </c>
       <c r="B558" t="str">
-        <v>George H. O'Brien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C558" t="str">
         <v>Physical medicine and rehabilitation at VA West Texas health care</v>
@@ -9871,7 +9871,7 @@
         <v>vha_519 - Polytrauma and traumatic brain injury</v>
       </c>
       <c r="B559" t="str">
-        <v>George H. O'Brien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C559" t="str">
         <v>Polytrauma and traumatic brain injury at VA West Texas health care</v>
@@ -9888,7 +9888,7 @@
         <v>vha_519 - Primary care</v>
       </c>
       <c r="B560" t="str">
-        <v>George H. O'Brien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C560" t="str">
         <v>Primary care at VA West Texas health care</v>
@@ -9905,7 +9905,7 @@
         <v>vha_519 - PTSD care</v>
       </c>
       <c r="B561" t="str">
-        <v>George H. O'Brien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C561" t="str">
         <v>PTSD care at VA West Texas health care</v>
@@ -9922,7 +9922,7 @@
         <v>vha_519 - Radiology</v>
       </c>
       <c r="B562" t="str">
-        <v>George H. O'Brien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C562" t="str">
         <v>Radiology at VA West Texas health care</v>
@@ -9939,7 +9939,7 @@
         <v>vha_519 - Returning service member care</v>
       </c>
       <c r="B563" t="str">
-        <v>George H. O'Brien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C563" t="str">
         <v>Returning service member care at VA West Texas health care</v>
@@ -9956,7 +9956,7 @@
         <v>vha_519 - Social work</v>
       </c>
       <c r="B564" t="str">
-        <v>George H. O'Brien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C564" t="str">
         <v>Social work at VA West Texas health care</v>
@@ -9973,7 +9973,7 @@
         <v>vha_519 - Spinal cord injury and disorders</v>
       </c>
       <c r="B565" t="str">
-        <v>George H. O'Brien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C565" t="str">
         <v>Spinal cord injury and disorders at VA West Texas health care</v>
@@ -9990,7 +9990,7 @@
         <v>vha_519 - Suicide prevention</v>
       </c>
       <c r="B566" t="str">
-        <v>George H. O'Brien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C566" t="str">
         <v>Suicide prevention at VA West Texas health care</v>
@@ -10007,7 +10007,7 @@
         <v>vha_519 - Telehealth</v>
       </c>
       <c r="B567" t="str">
-        <v>George H. O'Brien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C567" t="str">
         <v>Telehealth at VA West Texas health care</v>
@@ -10024,7 +10024,7 @@
         <v>vha_519 - Travel reimbursement</v>
       </c>
       <c r="B568" t="str">
-        <v>George H. O'Brien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C568" t="str">
         <v>Travel reimbursement at VA West Texas health care</v>
@@ -10041,7 +10041,7 @@
         <v>vha_519 - Vocational rehabilitation and employment programs</v>
       </c>
       <c r="B569" t="str">
-        <v>George H. O'Brien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C569" t="str">
         <v>Vocational rehabilitation and employment programs at VA West Texas health care</v>
@@ -10058,7 +10058,7 @@
         <v>vha_519 - Women Veteran care</v>
       </c>
       <c r="B570" t="str">
-        <v>George H. O'Brien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C570" t="str">
         <v>Women Veteran care at VA West Texas health care</v>

</xml_diff>

<commit_message>
Update remove apos to escape apos with "
</commit_message>
<xml_diff>
--- a/transformedFile.xlsx
+++ b/transformedFile.xlsx
@@ -1388,7 +1388,7 @@
         <v>vha_674 - Advice nurse</v>
       </c>
       <c r="B60" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C60" t="str">
         <v>Advice nurse at VA Central Texas health care</v>
@@ -1405,7 +1405,7 @@
         <v>vha_674 - Amputation care</v>
       </c>
       <c r="B61" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C61" t="str">
         <v>Amputation care at VA Central Texas health care</v>
@@ -1422,7 +1422,7 @@
         <v>vha_674 - Audiology and speech</v>
       </c>
       <c r="B62" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C62" t="str">
         <v>Audiology and speech at VA Central Texas health care</v>
@@ -1439,7 +1439,7 @@
         <v>vha_674 - Cardiology</v>
       </c>
       <c r="B63" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C63" t="str">
         <v>Cardiology at VA Central Texas health care</v>
@@ -1456,7 +1456,7 @@
         <v>vha_674 - Caregiver support</v>
       </c>
       <c r="B64" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C64" t="str">
         <v>Caregiver support at VA Central Texas health care</v>
@@ -1473,7 +1473,7 @@
         <v>vha_674 - Chiropractic</v>
       </c>
       <c r="B65" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C65" t="str">
         <v>Chiropractic at VA Central Texas health care</v>
@@ -1490,7 +1490,7 @@
         <v>vha_674 - Dental/oral surgery</v>
       </c>
       <c r="B66" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C66" t="str">
         <v>Dental/oral surgery at VA Central Texas health care</v>
@@ -1507,7 +1507,7 @@
         <v>vha_674 - Dermatology</v>
       </c>
       <c r="B67" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C67" t="str">
         <v>Dermatology at VA Central Texas health care</v>
@@ -1524,7 +1524,7 @@
         <v>vha_674 - Endocrinology</v>
       </c>
       <c r="B68" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C68" t="str">
         <v>Endocrinology at VA Central Texas health care</v>
@@ -1541,7 +1541,7 @@
         <v>vha_674 - Extended care and rehabilitation</v>
       </c>
       <c r="B69" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C69" t="str">
         <v>Extended care and rehabilitation at VA Central Texas health care</v>
@@ -1558,7 +1558,7 @@
         <v>vha_674 - Gastroenterology</v>
       </c>
       <c r="B70" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C70" t="str">
         <v>Gastroenterology at VA Central Texas health care</v>
@@ -1575,7 +1575,7 @@
         <v>vha_674 - Geriatrics</v>
       </c>
       <c r="B71" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C71" t="str">
         <v>Geriatrics at VA Central Texas health care</v>
@@ -1592,7 +1592,7 @@
         <v>vha_674 - Hematology/oncology</v>
       </c>
       <c r="B72" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C72" t="str">
         <v>Hematology/oncology at VA Central Texas health care</v>
@@ -1609,7 +1609,7 @@
         <v>vha_674 - Homeless Veteran care</v>
       </c>
       <c r="B73" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C73" t="str">
         <v>Homeless Veteran care at VA Central Texas health care</v>
@@ -1626,7 +1626,7 @@
         <v>vha_674 - Infectious disease</v>
       </c>
       <c r="B74" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C74" t="str">
         <v>Infectious disease at VA Central Texas health care</v>
@@ -1643,7 +1643,7 @@
         <v>vha_674 - Laboratory and pathology</v>
       </c>
       <c r="B75" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C75" t="str">
         <v>Laboratory and pathology at VA Central Texas health care</v>
@@ -1660,7 +1660,7 @@
         <v>vha_674 - LGBT Veteran care</v>
       </c>
       <c r="B76" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C76" t="str">
         <v>LGBT Veteran care at VA Central Texas health care</v>
@@ -1677,7 +1677,7 @@
         <v>vha_674 - Blind and low vision rehabilitation</v>
       </c>
       <c r="B77" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C77" t="str">
         <v>Blind and low vision rehabilitation at VA Central Texas health care</v>
@@ -1694,7 +1694,7 @@
         <v>vha_674 - Mental health care</v>
       </c>
       <c r="B78" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C78" t="str">
         <v>Mental health care at VA Central Texas health care</v>
@@ -1711,7 +1711,7 @@
         <v>vha_674 - Minority Veteran care</v>
       </c>
       <c r="B79" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C79" t="str">
         <v>Minority Veteran care at VA Central Texas health care</v>
@@ -1728,7 +1728,7 @@
         <v>vha_674 - MOVE! weight management</v>
       </c>
       <c r="B80" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C80" t="str">
         <v>MOVE! weight management at VA Central Texas health care</v>
@@ -1745,7 +1745,7 @@
         <v>vha_674 - My HealtheVet coordinator</v>
       </c>
       <c r="B81" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C81" t="str">
         <v>My HealtheVet coordinator at VA Central Texas health care</v>
@@ -1762,7 +1762,7 @@
         <v>vha_674 - Nephrology</v>
       </c>
       <c r="B82" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C82" t="str">
         <v>Nephrology at VA Central Texas health care</v>
@@ -1779,7 +1779,7 @@
         <v>vha_674 - Neurology</v>
       </c>
       <c r="B83" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C83" t="str">
         <v>Neurology at VA Central Texas health care</v>
@@ -1796,7 +1796,7 @@
         <v>vha_674 - Nutrition, food, and dietary care</v>
       </c>
       <c r="B84" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C84" t="str">
         <v>Nutrition, food, and dietary care at VA Central Texas health care</v>
@@ -1813,7 +1813,7 @@
         <v>vha_674 - Orthopedics</v>
       </c>
       <c r="B85" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C85" t="str">
         <v>Orthopedics at VA Central Texas health care</v>
@@ -1830,7 +1830,7 @@
         <v>vha_674 - Patient advocates</v>
       </c>
       <c r="B86" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C86" t="str">
         <v>Patient advocates at VA Central Texas health care</v>
@@ -1847,7 +1847,7 @@
         <v>vha_674 - Pharmacy</v>
       </c>
       <c r="B87" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C87" t="str">
         <v>Pharmacy at VA Central Texas health care</v>
@@ -1864,7 +1864,7 @@
         <v>vha_674 - Physical medicine and rehabilitation</v>
       </c>
       <c r="B88" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C88" t="str">
         <v>Physical medicine and rehabilitation at VA Central Texas health care</v>
@@ -1881,7 +1881,7 @@
         <v>vha_674 - Physical therapy, occupational therapy and kinesiotherapy</v>
       </c>
       <c r="B89" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C89" t="str">
         <v>Physical therapy, occupational therapy and kinesiotherapy at VA Central Texas health care</v>
@@ -1898,7 +1898,7 @@
         <v>vha_674 - Primary care</v>
       </c>
       <c r="B90" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C90" t="str">
         <v>Primary care at VA Central Texas health care</v>
@@ -1915,7 +1915,7 @@
         <v>vha_674 - Psychology</v>
       </c>
       <c r="B91" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C91" t="str">
         <v>Psychology at VA Central Texas health care</v>
@@ -1932,7 +1932,7 @@
         <v>vha_674 - PTSD care</v>
       </c>
       <c r="B92" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C92" t="str">
         <v>PTSD care at VA Central Texas health care</v>
@@ -1949,7 +1949,7 @@
         <v>vha_674 - Pulmonary medicine</v>
       </c>
       <c r="B93" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C93" t="str">
         <v>Pulmonary medicine at VA Central Texas health care</v>
@@ -1966,7 +1966,7 @@
         <v>vha_674 - Recreation and creative arts therapy</v>
       </c>
       <c r="B94" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C94" t="str">
         <v>Recreation and creative arts therapy at VA Central Texas health care</v>
@@ -1983,7 +1983,7 @@
         <v>vha_674 - Rehabilitation and prosthetics</v>
       </c>
       <c r="B95" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C95" t="str">
         <v>Rehabilitation and prosthetics at VA Central Texas health care</v>
@@ -2000,7 +2000,7 @@
         <v>vha_674 - Returning service member care</v>
       </c>
       <c r="B96" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C96" t="str">
         <v>Returning service member care at VA Central Texas health care</v>
@@ -2017,7 +2017,7 @@
         <v>vha_674 - Rheumatology</v>
       </c>
       <c r="B97" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C97" t="str">
         <v>Rheumatology at VA Central Texas health care</v>
@@ -2034,7 +2034,7 @@
         <v>vha_674 - Social work</v>
       </c>
       <c r="B98" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C98" t="str">
         <v>Social work at VA Central Texas health care</v>
@@ -2051,7 +2051,7 @@
         <v>vha_674 - Spinal cord injury and disorders</v>
       </c>
       <c r="B99" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C99" t="str">
         <v>Spinal cord injury and disorders at VA Central Texas health care</v>
@@ -2068,7 +2068,7 @@
         <v>vha_674 - Suicide prevention</v>
       </c>
       <c r="B100" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C100" t="str">
         <v>Suicide prevention at VA Central Texas health care</v>
@@ -2085,7 +2085,7 @@
         <v>vha_674 - Telehealth</v>
       </c>
       <c r="B101" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C101" t="str">
         <v>Telehealth at VA Central Texas health care</v>
@@ -2102,7 +2102,7 @@
         <v>vha_674 - Women Veteran care</v>
       </c>
       <c r="B102" t="str">
-        <v>Olin E. Teague Veterans Center</v>
+        <v>Olin E. Teague Veterans" Center</v>
       </c>
       <c r="C102" t="str">
         <v>Women Veteran care at VA Central Texas health care</v>
@@ -5434,7 +5434,7 @@
         <v>vha_671 - Allergy, asthma and immunology</v>
       </c>
       <c r="B298" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C298" t="str">
         <v>Allergy, asthma and immunology at VA South Texas health care</v>
@@ -5451,7 +5451,7 @@
         <v>vha_671 - Audiology and speech</v>
       </c>
       <c r="B299" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C299" t="str">
         <v>Audiology and speech at VA South Texas health care</v>
@@ -5468,7 +5468,7 @@
         <v>vha_671 - Cancer care</v>
       </c>
       <c r="B300" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C300" t="str">
         <v>Cancer care at VA South Texas health care</v>
@@ -5485,7 +5485,7 @@
         <v>vha_671 - Cardiology</v>
       </c>
       <c r="B301" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C301" t="str">
         <v>Cardiology at VA South Texas health care</v>
@@ -5502,7 +5502,7 @@
         <v>vha_671 - Caregiver support</v>
       </c>
       <c r="B302" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C302" t="str">
         <v>Caregiver support at VA South Texas health care</v>
@@ -5519,7 +5519,7 @@
         <v>vha_671 - Critical care</v>
       </c>
       <c r="B303" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C303" t="str">
         <v>Critical care at VA South Texas health care</v>
@@ -5536,7 +5536,7 @@
         <v>vha_671 - Dental/oral surgery</v>
       </c>
       <c r="B304" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C304" t="str">
         <v>Dental/oral surgery at VA South Texas health care</v>
@@ -5553,7 +5553,7 @@
         <v>vha_671 - Dermatology</v>
       </c>
       <c r="B305" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C305" t="str">
         <v>Dermatology at VA South Texas health care</v>
@@ -5570,7 +5570,7 @@
         <v>vha_671 - Endocrinology</v>
       </c>
       <c r="B306" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C306" t="str">
         <v>Endocrinology at VA South Texas health care</v>
@@ -5587,7 +5587,7 @@
         <v>vha_671 - Extended care and rehabilitation</v>
       </c>
       <c r="B307" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C307" t="str">
         <v>Extended care and rehabilitation at VA South Texas health care</v>
@@ -5604,7 +5604,7 @@
         <v>vha_671 - Gastroenterology</v>
       </c>
       <c r="B308" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C308" t="str">
         <v>Gastroenterology at VA South Texas health care</v>
@@ -5621,7 +5621,7 @@
         <v>vha_671 - Geriatrics</v>
       </c>
       <c r="B309" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C309" t="str">
         <v>Geriatrics at VA South Texas health care</v>
@@ -5638,7 +5638,7 @@
         <v>vha_671 - Hematology/oncology</v>
       </c>
       <c r="B310" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C310" t="str">
         <v>Hematology/oncology at VA South Texas health care</v>
@@ -5655,7 +5655,7 @@
         <v>vha_671 - Homeless Veteran care</v>
       </c>
       <c r="B311" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C311" t="str">
         <v>Homeless Veteran care at VA South Texas health care</v>
@@ -5672,7 +5672,7 @@
         <v>vha_671 - Infectious disease</v>
       </c>
       <c r="B312" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C312" t="str">
         <v>Infectious disease at VA South Texas health care</v>
@@ -5689,7 +5689,7 @@
         <v>vha_671 - LGBT Veteran care</v>
       </c>
       <c r="B313" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C313" t="str">
         <v>LGBT Veteran care at VA South Texas health care</v>
@@ -5706,7 +5706,7 @@
         <v>vha_671 - Blind and low vision rehabilitation</v>
       </c>
       <c r="B314" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C314" t="str">
         <v>Blind and low vision rehabilitation at VA South Texas health care</v>
@@ -5723,7 +5723,7 @@
         <v>vha_671 - Mental health care</v>
       </c>
       <c r="B315" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C315" t="str">
         <v>Mental health care at VA South Texas health care</v>
@@ -5740,7 +5740,7 @@
         <v>vha_671 - Military sexual trauma care</v>
       </c>
       <c r="B316" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C316" t="str">
         <v>Military sexual trauma care at VA South Texas health care</v>
@@ -5757,7 +5757,7 @@
         <v>vha_671 - Minority Veteran care</v>
       </c>
       <c r="B317" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C317" t="str">
         <v>Minority Veteran care at VA South Texas health care</v>
@@ -5774,7 +5774,7 @@
         <v>vha_671 - MOVE! weight management</v>
       </c>
       <c r="B318" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C318" t="str">
         <v>MOVE! weight management at VA South Texas health care</v>
@@ -5791,7 +5791,7 @@
         <v>vha_671 - Nephrology</v>
       </c>
       <c r="B319" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C319" t="str">
         <v>Nephrology at VA South Texas health care</v>
@@ -5808,7 +5808,7 @@
         <v>vha_671 - Neurology</v>
       </c>
       <c r="B320" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C320" t="str">
         <v>Neurology at VA South Texas health care</v>
@@ -5825,7 +5825,7 @@
         <v>vha_671 - Palliative and hospice care</v>
       </c>
       <c r="B321" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C321" t="str">
         <v>Palliative and hospice care at VA South Texas health care</v>
@@ -5842,7 +5842,7 @@
         <v>vha_671 - Patient advocates</v>
       </c>
       <c r="B322" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C322" t="str">
         <v>Patient advocates at VA South Texas health care</v>
@@ -5859,7 +5859,7 @@
         <v>vha_671 - Pharmacy</v>
       </c>
       <c r="B323" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C323" t="str">
         <v>Pharmacy at VA South Texas health care</v>
@@ -5876,7 +5876,7 @@
         <v>vha_671 - Physical medicine and rehabilitation</v>
       </c>
       <c r="B324" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C324" t="str">
         <v>Physical medicine and rehabilitation at VA South Texas health care</v>
@@ -5893,7 +5893,7 @@
         <v>vha_671 - Polytrauma and traumatic brain injury</v>
       </c>
       <c r="B325" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C325" t="str">
         <v>Polytrauma and traumatic brain injury at VA South Texas health care</v>
@@ -5910,7 +5910,7 @@
         <v>vha_671 - Primary care</v>
       </c>
       <c r="B326" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C326" t="str">
         <v>Primary care at VA South Texas health care</v>
@@ -5927,7 +5927,7 @@
         <v>vha_671 - Pulmonary medicine</v>
       </c>
       <c r="B327" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C327" t="str">
         <v>Pulmonary medicine at VA South Texas health care</v>
@@ -5944,7 +5944,7 @@
         <v>vha_671 - Rehabilitation and prosthetics</v>
       </c>
       <c r="B328" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C328" t="str">
         <v>Rehabilitation and prosthetics at VA South Texas health care</v>
@@ -5961,7 +5961,7 @@
         <v>vha_671 - Returning service member care</v>
       </c>
       <c r="B329" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C329" t="str">
         <v>Returning service member care at VA South Texas health care</v>
@@ -5978,7 +5978,7 @@
         <v>vha_671 - Rheumatology</v>
       </c>
       <c r="B330" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C330" t="str">
         <v>Rheumatology at VA South Texas health care</v>
@@ -5995,7 +5995,7 @@
         <v>vha_671 - Sleep medicine</v>
       </c>
       <c r="B331" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C331" t="str">
         <v>Sleep medicine at VA South Texas health care</v>
@@ -6012,7 +6012,7 @@
         <v>vha_671 - Social work</v>
       </c>
       <c r="B332" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C332" t="str">
         <v>Social work at VA South Texas health care</v>
@@ -6029,7 +6029,7 @@
         <v>vha_671 - Suicide prevention</v>
       </c>
       <c r="B333" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C333" t="str">
         <v>Suicide prevention at VA South Texas health care</v>
@@ -6046,7 +6046,7 @@
         <v>vha_671 - Telehealth</v>
       </c>
       <c r="B334" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C334" t="str">
         <v>Telehealth at VA South Texas health care</v>
@@ -6063,7 +6063,7 @@
         <v>vha_671 - Transplant surgery</v>
       </c>
       <c r="B335" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C335" t="str">
         <v>Transplant surgery at VA South Texas health care</v>
@@ -6080,7 +6080,7 @@
         <v>vha_671 - Vocational rehabilitation and employment programs</v>
       </c>
       <c r="B336" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C336" t="str">
         <v>Vocational rehabilitation and employment programs at VA South Texas health care</v>
@@ -6097,7 +6097,7 @@
         <v>vha_671 - Women Veteran care</v>
       </c>
       <c r="B337" t="str">
-        <v>Audie L. Murphy Memorial Veterans Hospital</v>
+        <v>Audie L. Murphy Memorial Veterans" Hospital</v>
       </c>
       <c r="C337" t="str">
         <v>Women Veteran care at VA South Texas health care</v>
@@ -9582,7 +9582,7 @@
         <v>vha_519 - Addiction and substance abuse care</v>
       </c>
       <c r="B542" t="str">
-        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. O"Brien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C542" t="str">
         <v>Addiction and substance abuse care at VA West Texas health care</v>
@@ -9599,7 +9599,7 @@
         <v>vha_519 - Advice nurse</v>
       </c>
       <c r="B543" t="str">
-        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. O"Brien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C543" t="str">
         <v>Advice nurse at VA West Texas health care</v>
@@ -9616,7 +9616,7 @@
         <v>vha_519 - Audiology and speech</v>
       </c>
       <c r="B544" t="str">
-        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. O"Brien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C544" t="str">
         <v>Audiology and speech at VA West Texas health care</v>
@@ -9633,7 +9633,7 @@
         <v>vha_519 - Caregiver support</v>
       </c>
       <c r="B545" t="str">
-        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. O"Brien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C545" t="str">
         <v>Caregiver support at VA West Texas health care</v>
@@ -9650,7 +9650,7 @@
         <v>vha_519 - Dental/oral surgery</v>
       </c>
       <c r="B546" t="str">
-        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. O"Brien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C546" t="str">
         <v>Dental/oral surgery at VA West Texas health care</v>
@@ -9667,7 +9667,7 @@
         <v>vha_519 - Extended care and rehabilitation</v>
       </c>
       <c r="B547" t="str">
-        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. O"Brien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C547" t="str">
         <v>Extended care and rehabilitation at VA West Texas health care</v>
@@ -9684,7 +9684,7 @@
         <v>vha_519 - Homeless Veteran care</v>
       </c>
       <c r="B548" t="str">
-        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. O"Brien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C548" t="str">
         <v>Homeless Veteran care at VA West Texas health care</v>
@@ -9701,7 +9701,7 @@
         <v>vha_519 - Laboratory and pathology</v>
       </c>
       <c r="B549" t="str">
-        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. O"Brien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C549" t="str">
         <v>Laboratory and pathology at VA West Texas health care</v>
@@ -9718,7 +9718,7 @@
         <v>vha_519 - LGBT Veteran care</v>
       </c>
       <c r="B550" t="str">
-        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. O"Brien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C550" t="str">
         <v>LGBT Veteran care at VA West Texas health care</v>
@@ -9735,7 +9735,7 @@
         <v>vha_519 - Mental health care</v>
       </c>
       <c r="B551" t="str">
-        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. O"Brien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C551" t="str">
         <v>Mental health care at VA West Texas health care</v>
@@ -9752,7 +9752,7 @@
         <v>vha_519 - Minority Veteran care</v>
       </c>
       <c r="B552" t="str">
-        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. O"Brien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C552" t="str">
         <v>Minority Veteran care at VA West Texas health care</v>
@@ -9769,7 +9769,7 @@
         <v>vha_519 - Nutrition, food, and dietary care</v>
       </c>
       <c r="B553" t="str">
-        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. O"Brien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C553" t="str">
         <v>Nutrition, food, and dietary care at VA West Texas health care</v>
@@ -9786,7 +9786,7 @@
         <v>vha_519 - Ophthalmology</v>
       </c>
       <c r="B554" t="str">
-        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. O"Brien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C554" t="str">
         <v>Ophthalmology at VA West Texas health care</v>
@@ -9803,7 +9803,7 @@
         <v>vha_519 - Palliative and hospice care</v>
       </c>
       <c r="B555" t="str">
-        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. O"Brien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C555" t="str">
         <v>Palliative and hospice care at VA West Texas health care</v>
@@ -9820,7 +9820,7 @@
         <v>vha_519 - Patient advocates</v>
       </c>
       <c r="B556" t="str">
-        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. O"Brien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C556" t="str">
         <v>Patient advocates at VA West Texas health care</v>
@@ -9837,7 +9837,7 @@
         <v>vha_519 - Pharmacy</v>
       </c>
       <c r="B557" t="str">
-        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. O"Brien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C557" t="str">
         <v>Pharmacy at VA West Texas health care</v>
@@ -9854,7 +9854,7 @@
         <v>vha_519 - Physical medicine and rehabilitation</v>
       </c>
       <c r="B558" t="str">
-        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. O"Brien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C558" t="str">
         <v>Physical medicine and rehabilitation at VA West Texas health care</v>
@@ -9871,7 +9871,7 @@
         <v>vha_519 - Polytrauma and traumatic brain injury</v>
       </c>
       <c r="B559" t="str">
-        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. O"Brien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C559" t="str">
         <v>Polytrauma and traumatic brain injury at VA West Texas health care</v>
@@ -9888,7 +9888,7 @@
         <v>vha_519 - Primary care</v>
       </c>
       <c r="B560" t="str">
-        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. O"Brien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C560" t="str">
         <v>Primary care at VA West Texas health care</v>
@@ -9905,7 +9905,7 @@
         <v>vha_519 - PTSD care</v>
       </c>
       <c r="B561" t="str">
-        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. O"Brien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C561" t="str">
         <v>PTSD care at VA West Texas health care</v>
@@ -9922,7 +9922,7 @@
         <v>vha_519 - Radiology</v>
       </c>
       <c r="B562" t="str">
-        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. O"Brien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C562" t="str">
         <v>Radiology at VA West Texas health care</v>
@@ -9939,7 +9939,7 @@
         <v>vha_519 - Returning service member care</v>
       </c>
       <c r="B563" t="str">
-        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. O"Brien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C563" t="str">
         <v>Returning service member care at VA West Texas health care</v>
@@ -9956,7 +9956,7 @@
         <v>vha_519 - Social work</v>
       </c>
       <c r="B564" t="str">
-        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. O"Brien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C564" t="str">
         <v>Social work at VA West Texas health care</v>
@@ -9973,7 +9973,7 @@
         <v>vha_519 - Spinal cord injury and disorders</v>
       </c>
       <c r="B565" t="str">
-        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. O"Brien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C565" t="str">
         <v>Spinal cord injury and disorders at VA West Texas health care</v>
@@ -9990,7 +9990,7 @@
         <v>vha_519 - Suicide prevention</v>
       </c>
       <c r="B566" t="str">
-        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. O"Brien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C566" t="str">
         <v>Suicide prevention at VA West Texas health care</v>
@@ -10007,7 +10007,7 @@
         <v>vha_519 - Telehealth</v>
       </c>
       <c r="B567" t="str">
-        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. O"Brien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C567" t="str">
         <v>Telehealth at VA West Texas health care</v>
@@ -10024,7 +10024,7 @@
         <v>vha_519 - Travel reimbursement</v>
       </c>
       <c r="B568" t="str">
-        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. O"Brien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C568" t="str">
         <v>Travel reimbursement at VA West Texas health care</v>
@@ -10041,7 +10041,7 @@
         <v>vha_519 - Vocational rehabilitation and employment programs</v>
       </c>
       <c r="B569" t="str">
-        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. O"Brien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C569" t="str">
         <v>Vocational rehabilitation and employment programs at VA West Texas health care</v>
@@ -10058,7 +10058,7 @@
         <v>vha_519 - Women Veteran care</v>
       </c>
       <c r="B570" t="str">
-        <v>George H. OBrien, Jr. Department of Veterans Affairs Medical Center</v>
+        <v>George H. O"Brien, Jr. Department of Veterans Affairs Medical Center</v>
       </c>
       <c r="C570" t="str">
         <v>Women Veteran care at VA West Texas health care</v>

</xml_diff>